<commit_message>
Version 5 envío de archivo con mensaje de correo
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/REGISTRO XXIII_TESTMAIL.xlsx
+++ b/Archivos de trabajo/REGISTRO XXIII_TESTMAIL.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="469">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -252,21 +252,12 @@
     <t>Lizama</t>
   </si>
   <si>
-    <t>Cruz</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>Lozano</t>
   </si>
   <si>
     <t>Reyes</t>
   </si>
   <si>
-    <t>Gutiérrez</t>
-  </si>
-  <si>
     <t>Preparatoria 16</t>
   </si>
   <si>
@@ -405,12 +396,6 @@
     <t>Rodriguez</t>
   </si>
   <si>
-    <t>Rivera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mendoza </t>
-  </si>
-  <si>
     <t>Lara</t>
   </si>
   <si>
@@ -1167,66 +1152,24 @@
     <t>Diego Emilio</t>
   </si>
   <si>
-    <t xml:space="preserve">Santiago </t>
-  </si>
-  <si>
-    <t>Fuentes</t>
-  </si>
-  <si>
     <t>Colegio Salesianos Don Bosco de Monterrey</t>
   </si>
   <si>
-    <t>Linux DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verónica </t>
-  </si>
-  <si>
     <t>Bulos</t>
   </si>
   <si>
-    <t>Treviño</t>
-  </si>
-  <si>
-    <t>María Fernanda</t>
-  </si>
-  <si>
-    <t>fernanda.treviñogt@uanl.edu,mx</t>
-  </si>
-  <si>
     <t>Pedraza</t>
   </si>
   <si>
-    <t>Alondra Esther</t>
-  </si>
-  <si>
-    <t>alondra.guerrerop@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>Lucio</t>
-  </si>
-  <si>
-    <t>Marisol Carolina</t>
-  </si>
-  <si>
-    <t>carolina.riveral@uanl.edu.mx</t>
-  </si>
-  <si>
     <t>Díaz</t>
   </si>
   <si>
     <t>Baez</t>
   </si>
   <si>
-    <t>Debanhi Elizabeth</t>
-  </si>
-  <si>
     <t>debanhi.diazb@uanl.edu.mx</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1YcWD3BnFwncN5QEwNCQ4HUu7_z9S6HEC</t>
-  </si>
-  <si>
     <t>Androides DB</t>
   </si>
   <si>
@@ -1275,114 +1218,15 @@
     <t>https://drive.google.com/open?id=1YCm9pIG0Tjg9bKqPTezhfl7eBKIfM4RR</t>
   </si>
   <si>
-    <t>Preparatoria 1</t>
-  </si>
-  <si>
-    <t>Jerry's.exe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jesús Erick Mauricio </t>
   </si>
   <si>
     <t xml:space="preserve">Palacios </t>
   </si>
   <si>
-    <t xml:space="preserve">Hernández </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aranza </t>
-  </si>
-  <si>
-    <t>aranza.santiagoh@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loera </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daira Giselle </t>
-  </si>
-  <si>
-    <t>giselle.loeram@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puente </t>
-  </si>
-  <si>
-    <t>Axel Haziel</t>
-  </si>
-  <si>
-    <t>haziel.rodriguezp@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Briones </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aguayo </t>
-  </si>
-  <si>
-    <t>Cynthia Mayrin</t>
-  </si>
-  <si>
-    <t>cynthia.brionesa@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1pMoAhBvMbxGa0wxY8UUUiJwXj6QOiO09</t>
-  </si>
-  <si>
-    <t>Diablillos</t>
-  </si>
-  <si>
-    <t>Jesus Erick Mauricio</t>
-  </si>
-  <si>
-    <t>Palacios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gómez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alonso </t>
-  </si>
-  <si>
-    <t>Joshua Alain</t>
-  </si>
-  <si>
-    <t>joshua.gomeza@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>del Angel</t>
-  </si>
-  <si>
     <t>Antonio</t>
   </si>
   <si>
-    <t>Brenda Janeth</t>
-  </si>
-  <si>
-    <t>brenda.dela@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leija </t>
-  </si>
-  <si>
-    <t>Zaragoza</t>
-  </si>
-  <si>
-    <t>Angel Alberto</t>
-  </si>
-  <si>
-    <t>angel.leijaz@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osvaldo Daniel </t>
-  </si>
-  <si>
-    <t>osvaldo.trevinof@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1OWyWEvCgZC5uBAgc_qRIMRVymRABi_Ym</t>
-  </si>
-  <si>
     <t xml:space="preserve">Juan Antonio </t>
   </si>
   <si>
@@ -1392,139 +1236,25 @@
     <t xml:space="preserve">Jahir Antonio </t>
   </si>
   <si>
-    <t>Preparatoria 13</t>
-  </si>
-  <si>
-    <t>ResQbot</t>
-  </si>
-  <si>
     <t>Tamez</t>
   </si>
   <si>
     <t>Tapia</t>
   </si>
   <si>
-    <t>Chávez</t>
-  </si>
-  <si>
-    <t>Estudillo</t>
-  </si>
-  <si>
-    <t>Emiliano</t>
-  </si>
-  <si>
-    <t>emiliano.chaveze@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>emiliano.torrescr@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>Dylan Yitzhak</t>
-  </si>
-  <si>
-    <t>yitzhak.martinezs@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1klLbXuQ4SkHygiTdMlBZE_Wb44EMH-Hs</t>
-  </si>
-  <si>
-    <t>Preparatoria 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boxeadores </t>
-  </si>
-  <si>
     <t xml:space="preserve">Víctor Manuel </t>
   </si>
   <si>
     <t>Hiracheta</t>
   </si>
   <si>
-    <t>Quiroz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guadalupe Rafael </t>
-  </si>
-  <si>
-    <t>rafaelquirozl@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jesús </t>
-  </si>
-  <si>
-    <t>jesus.garzaflr@uaml.edu.mx</t>
-  </si>
-  <si>
-    <t>Zamora</t>
-  </si>
-  <si>
-    <t>Gael Mariano</t>
-  </si>
-  <si>
-    <t>gael.zamoral@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uriegas </t>
-  </si>
-  <si>
-    <t>Miramontes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabián </t>
-  </si>
-  <si>
-    <t>fabian.uriegasm@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=13skxUNCS1Vtad26JWmP44CwpQAeCdIks</t>
-  </si>
-  <si>
     <t>Jorge Adolfo</t>
   </si>
   <si>
-    <t>Escuela Industrial y Preparatoria Técnica Álvaro Obregón</t>
-  </si>
-  <si>
-    <t>Dogotics</t>
-  </si>
-  <si>
     <t>Rafael Alfredo</t>
   </si>
   <si>
     <t>Cavazos</t>
-  </si>
-  <si>
-    <t>Valero</t>
-  </si>
-  <si>
-    <t>jesus.hernandezvlr@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>Gabriela Jocelyn</t>
-  </si>
-  <si>
-    <t>gabriela.garciarc@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huerta </t>
-  </si>
-  <si>
-    <t>Aquiles Gibran</t>
-  </si>
-  <si>
-    <t>aquiles.huertar@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>Lázaro</t>
-  </si>
-  <si>
-    <t>José</t>
-  </si>
-  <si>
-    <t>jose.morenolzr@uanl.edu.mx</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=19u5UKQqmbGsdHY-uCxhMEFUnY66BEuMx</t>
   </si>
   <si>
     <t>Karla Alejandra</t>
@@ -2180,7 +1910,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2357,40 +2087,40 @@
         <v>46069.845060509258</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>414</v>
       </c>
       <c r="D2" t="s">
-        <v>523</v>
+        <v>433</v>
       </c>
       <c r="E2" t="s">
         <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>524</v>
+        <v>434</v>
       </c>
       <c r="G2" t="s">
-        <v>525</v>
+        <v>435</v>
       </c>
       <c r="H2" t="s">
-        <v>508</v>
+        <v>418</v>
       </c>
       <c r="I2">
         <v>8111189542</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
       <c r="K2">
         <v>2229925</v>
       </c>
       <c r="L2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>526</v>
+        <v>436</v>
       </c>
       <c r="O2" t="s">
         <v>52</v>
@@ -2399,19 +2129,19 @@
         <v>39971</v>
       </c>
       <c r="Q2" t="s">
-        <v>527</v>
+        <v>437</v>
       </c>
       <c r="R2">
         <v>2229923</v>
       </c>
       <c r="S2" t="s">
-        <v>528</v>
+        <v>438</v>
       </c>
       <c r="T2" t="s">
-        <v>529</v>
+        <v>439</v>
       </c>
       <c r="U2" t="s">
-        <v>530</v>
+        <v>440</v>
       </c>
       <c r="V2" t="s">
         <v>52</v>
@@ -2420,19 +2150,19 @@
         <v>40075</v>
       </c>
       <c r="X2" t="s">
-        <v>531</v>
+        <v>441</v>
       </c>
       <c r="Y2">
         <v>2229454</v>
       </c>
       <c r="Z2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AA2" t="s">
-        <v>532</v>
+        <v>442</v>
       </c>
       <c r="AB2" t="s">
-        <v>533</v>
+        <v>443</v>
       </c>
       <c r="AC2" t="s">
         <v>52</v>
@@ -2441,19 +2171,19 @@
         <v>39907</v>
       </c>
       <c r="AE2" t="s">
-        <v>534</v>
+        <v>444</v>
       </c>
       <c r="AF2">
         <v>2279143</v>
       </c>
       <c r="AG2" t="s">
-        <v>535</v>
+        <v>445</v>
       </c>
       <c r="AH2" t="s">
-        <v>536</v>
+        <v>446</v>
       </c>
       <c r="AI2" t="s">
-        <v>537</v>
+        <v>447</v>
       </c>
       <c r="AJ2" t="s">
         <v>59</v>
@@ -2462,7 +2192,7 @@
         <v>40254</v>
       </c>
       <c r="AL2" t="s">
-        <v>538</v>
+        <v>448</v>
       </c>
       <c r="AM2" t="s">
         <v>60</v>
@@ -2471,13 +2201,13 @@
         <v>2279353</v>
       </c>
       <c r="AO2" t="s">
-        <v>539</v>
+        <v>449</v>
       </c>
       <c r="AP2" t="s">
-        <v>540</v>
+        <v>450</v>
       </c>
       <c r="AQ2" t="s">
-        <v>541</v>
+        <v>451</v>
       </c>
       <c r="AR2" t="s">
         <v>59</v>
@@ -2486,10 +2216,10 @@
         <v>40187</v>
       </c>
       <c r="AT2" t="s">
-        <v>542</v>
+        <v>452</v>
       </c>
       <c r="AU2" t="s">
-        <v>543</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2497,40 +2227,40 @@
         <v>46069.848373773144</v>
       </c>
       <c r="B3" t="s">
-        <v>504</v>
+        <v>414</v>
       </c>
       <c r="D3" t="s">
-        <v>544</v>
+        <v>454</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>506</v>
+        <v>416</v>
       </c>
       <c r="G3" t="s">
-        <v>507</v>
+        <v>417</v>
       </c>
       <c r="H3" t="s">
-        <v>503</v>
+        <v>413</v>
       </c>
       <c r="I3">
         <v>8111189542</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
       <c r="K3">
         <v>2229604</v>
       </c>
       <c r="L3" t="s">
-        <v>457</v>
+        <v>403</v>
       </c>
       <c r="M3" t="s">
-        <v>545</v>
+        <v>455</v>
       </c>
       <c r="N3" t="s">
-        <v>546</v>
+        <v>456</v>
       </c>
       <c r="O3" t="s">
         <v>52</v>
@@ -2539,7 +2269,7 @@
         <v>39955</v>
       </c>
       <c r="Q3" t="s">
-        <v>547</v>
+        <v>457</v>
       </c>
       <c r="R3">
         <v>2229971</v>
@@ -2551,7 +2281,7 @@
         <v>69</v>
       </c>
       <c r="U3" t="s">
-        <v>548</v>
+        <v>458</v>
       </c>
       <c r="V3" t="s">
         <v>52</v>
@@ -2560,19 +2290,19 @@
         <v>39899</v>
       </c>
       <c r="X3" t="s">
-        <v>549</v>
+        <v>459</v>
       </c>
       <c r="Y3">
         <v>2278807</v>
       </c>
       <c r="Z3" t="s">
-        <v>550</v>
+        <v>460</v>
       </c>
       <c r="AA3" t="s">
-        <v>551</v>
+        <v>461</v>
       </c>
       <c r="AB3" t="s">
-        <v>552</v>
+        <v>462</v>
       </c>
       <c r="AC3" t="s">
         <v>59</v>
@@ -2581,19 +2311,19 @@
         <v>40451</v>
       </c>
       <c r="AE3" t="s">
-        <v>553</v>
+        <v>463</v>
       </c>
       <c r="AF3">
         <v>2279588</v>
       </c>
       <c r="AG3" t="s">
-        <v>554</v>
+        <v>464</v>
       </c>
       <c r="AH3" t="s">
         <v>58</v>
       </c>
       <c r="AI3" t="s">
-        <v>453</v>
+        <v>401</v>
       </c>
       <c r="AJ3" t="s">
         <v>59</v>
@@ -2602,13 +2332,13 @@
         <v>40188</v>
       </c>
       <c r="AL3" t="s">
-        <v>555</v>
+        <v>465</v>
       </c>
       <c r="AM3" t="s">
         <v>54</v>
       </c>
       <c r="AU3" t="s">
-        <v>556</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2616,40 +2346,40 @@
         <v>46069.833987974533</v>
       </c>
       <c r="B4" t="s">
-        <v>504</v>
+        <v>414</v>
       </c>
       <c r="D4" t="s">
-        <v>505</v>
+        <v>415</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>506</v>
+        <v>416</v>
       </c>
       <c r="G4" t="s">
-        <v>507</v>
+        <v>417</v>
       </c>
       <c r="H4" t="s">
-        <v>508</v>
+        <v>418</v>
       </c>
       <c r="I4">
         <v>8111189542</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
       <c r="K4">
         <v>2229836</v>
       </c>
       <c r="L4" t="s">
-        <v>509</v>
+        <v>419</v>
       </c>
       <c r="M4" t="s">
         <v>70</v>
       </c>
       <c r="N4" t="s">
-        <v>510</v>
+        <v>420</v>
       </c>
       <c r="O4" t="s">
         <v>52</v>
@@ -2658,19 +2388,19 @@
         <v>40010</v>
       </c>
       <c r="Q4" t="s">
-        <v>511</v>
+        <v>421</v>
       </c>
       <c r="R4">
         <v>2229446</v>
       </c>
       <c r="S4" t="s">
-        <v>512</v>
+        <v>422</v>
       </c>
       <c r="T4" t="s">
-        <v>513</v>
+        <v>423</v>
       </c>
       <c r="U4" t="s">
-        <v>514</v>
+        <v>424</v>
       </c>
       <c r="V4" t="s">
         <v>52</v>
@@ -2679,19 +2409,19 @@
         <v>39865</v>
       </c>
       <c r="X4" t="s">
-        <v>515</v>
+        <v>425</v>
       </c>
       <c r="Y4">
         <v>2305375</v>
       </c>
       <c r="Z4" t="s">
-        <v>516</v>
+        <v>426</v>
       </c>
       <c r="AA4" t="s">
-        <v>517</v>
+        <v>427</v>
       </c>
       <c r="AB4" t="s">
-        <v>518</v>
+        <v>428</v>
       </c>
       <c r="AC4" t="s">
         <v>59</v>
@@ -2700,19 +2430,19 @@
         <v>40275</v>
       </c>
       <c r="AE4" t="s">
-        <v>519</v>
+        <v>429</v>
       </c>
       <c r="AF4">
         <v>2279527</v>
       </c>
       <c r="AG4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AH4" t="s">
         <v>61</v>
       </c>
       <c r="AI4" t="s">
-        <v>520</v>
+        <v>430</v>
       </c>
       <c r="AJ4" t="s">
         <v>59</v>
@@ -2721,13 +2451,13 @@
         <v>40422</v>
       </c>
       <c r="AL4" t="s">
-        <v>521</v>
+        <v>431</v>
       </c>
       <c r="AM4" t="s">
         <v>54</v>
       </c>
       <c r="AU4" t="s">
-        <v>522</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2735,82 +2465,82 @@
         <v>46066.514186412038</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I5" s="2">
         <v>8116218385</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
       <c r="K5" s="2">
         <v>2220193</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P5" s="3">
         <v>39486</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="R5" s="2">
         <v>2220134</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W5" s="3">
         <v>39746</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="Y5" s="2">
         <v>2268862</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AC5" s="2" t="s">
         <v>52</v>
@@ -2819,19 +2549,19 @@
         <v>39942</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AF5" s="2">
         <v>2268855</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="AJ5" s="2" t="s">
         <v>52</v>
@@ -2840,13 +2570,13 @@
         <v>39810</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="AM5" s="2" t="s">
         <v>54</v>
       </c>
       <c r="AU5" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2854,40 +2584,40 @@
         <v>46068.630102314812</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I6" s="2">
         <v>7731633931</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>558</v>
+        <v>468</v>
       </c>
       <c r="K6" s="2">
         <v>2268256</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>52</v>
@@ -2896,19 +2626,19 @@
         <v>39603</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="R6" s="2">
         <v>2268259</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>52</v>
@@ -2917,7 +2647,7 @@
         <v>40046</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="Y6" s="2">
         <v>2268237</v>
@@ -2926,10 +2656,10 @@
         <v>49</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="AC6" s="2" t="s">
         <v>52</v>
@@ -2938,25 +2668,25 @@
         <v>39835</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="AF6" s="2">
         <v>2268244</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="AJ6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="AM6" s="2" t="s">
         <v>60</v>
@@ -2965,13 +2695,13 @@
         <v>2268244</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="AR6" s="2" t="s">
         <v>52</v>
@@ -2980,704 +2710,143 @@
         <v>40157</v>
       </c>
       <c r="AT6" s="2" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>46068.618912199076</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I7" s="2">
-        <v>7731633931</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2319787</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="3">
-        <v>40430</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="R7" s="2">
-        <v>2319792</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="W7" s="3">
-        <v>40411</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>2319814</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>40416</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN7" s="2">
-        <v>2268256</v>
-      </c>
-      <c r="AO7" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="AQ7" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="AR7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS7" s="3">
-        <v>39603</v>
-      </c>
-      <c r="AT7" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="AU7" s="4" t="s">
-        <v>399</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="4"/>
     </row>
     <row r="8" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>46069.736656134264</v>
-      </c>
-      <c r="B8" t="s">
-        <v>485</v>
-      </c>
-      <c r="D8" t="s">
-        <v>486</v>
-      </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" t="s">
-        <v>487</v>
-      </c>
-      <c r="G8" t="s">
-        <v>488</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8">
-        <v>8115193174</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K8">
-        <v>2251387</v>
-      </c>
-      <c r="L8" t="s">
-        <v>173</v>
-      </c>
-      <c r="M8" t="s">
-        <v>489</v>
-      </c>
-      <c r="N8" t="s">
-        <v>130</v>
-      </c>
-      <c r="O8" t="s">
-        <v>52</v>
-      </c>
-      <c r="P8">
-        <v>40066</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>490</v>
-      </c>
-      <c r="R8">
-        <v>2295970</v>
-      </c>
-      <c r="S8" t="s">
-        <v>131</v>
-      </c>
-      <c r="T8" t="s">
-        <v>290</v>
-      </c>
-      <c r="U8" t="s">
-        <v>491</v>
-      </c>
-      <c r="V8" t="s">
-        <v>59</v>
-      </c>
-      <c r="W8">
-        <v>40418</v>
-      </c>
-      <c r="X8" t="s">
-        <v>492</v>
-      </c>
-      <c r="Y8">
-        <v>2295656</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>493</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>494</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD8">
-        <v>40441</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>495</v>
-      </c>
-      <c r="AF8">
-        <v>2294977</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>204</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>496</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>497</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK8">
-        <v>40318</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>498</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>499</v>
-      </c>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>46069.407399768519</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="2">
-        <v>8186894656</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2281424</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="3">
-        <v>40223</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="R9" s="2">
-        <v>2281079</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="W9" s="3">
-        <v>40506</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>2280020</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD9" s="3">
-        <v>40476</v>
-      </c>
-      <c r="AE9" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>2280871</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="AH9" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="AJ9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK9" s="3">
-        <v>40324</v>
-      </c>
-      <c r="AL9" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="AM9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU9" s="4" t="s">
-        <v>433</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AU9" s="4"/>
     </row>
     <row r="10" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>46069.411885173613</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I10" s="2">
-        <v>8186894656</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K10" s="2">
-        <v>2281479</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="3">
-        <v>40517</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="R10" s="2">
-        <v>2280272</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="W10" s="3">
-        <v>40225</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>2282137</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD10" s="3">
-        <v>39614</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>2280413</v>
-      </c>
-      <c r="AG10" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="AH10" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="AI10" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="AJ10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK10" s="3">
-        <v>40231</v>
-      </c>
-      <c r="AL10" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="AM10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU10" s="4" t="s">
-        <v>451</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AU10" s="4"/>
     </row>
     <row r="11" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>46069.678112881942</v>
-      </c>
-      <c r="B11" t="s">
-        <v>455</v>
-      </c>
-      <c r="D11" t="s">
-        <v>456</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>442</v>
-      </c>
-      <c r="G11" t="s">
-        <v>457</v>
-      </c>
-      <c r="H11" t="s">
-        <v>458</v>
-      </c>
-      <c r="I11">
-        <v>8110104654</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K11">
-        <v>2258835</v>
-      </c>
-      <c r="L11" t="s">
-        <v>459</v>
-      </c>
-      <c r="M11" t="s">
-        <v>460</v>
-      </c>
-      <c r="N11" t="s">
-        <v>461</v>
-      </c>
-      <c r="O11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11">
-        <v>40172</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>462</v>
-      </c>
-      <c r="R11">
-        <v>2258897</v>
-      </c>
-      <c r="S11" t="s">
-        <v>124</v>
-      </c>
-      <c r="T11" t="s">
-        <v>75</v>
-      </c>
-      <c r="U11" t="s">
-        <v>461</v>
-      </c>
-      <c r="V11" t="s">
-        <v>52</v>
-      </c>
-      <c r="W11">
-        <v>39861</v>
-      </c>
-      <c r="X11" t="s">
-        <v>463</v>
-      </c>
-      <c r="Y11">
-        <v>2258825</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>464</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD11">
-        <v>39925</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>465</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>466</v>
-      </c>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>46069.68214478009</v>
-      </c>
-      <c r="B12" t="s">
-        <v>467</v>
-      </c>
-      <c r="D12" t="s">
-        <v>468</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>469</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>470</v>
-      </c>
-      <c r="I12">
-        <v>8261168486</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="K12">
-        <v>2259133</v>
-      </c>
-      <c r="L12" t="s">
-        <v>471</v>
-      </c>
-      <c r="M12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" t="s">
-        <v>472</v>
-      </c>
-      <c r="O12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12">
-        <v>40103</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>473</v>
-      </c>
-      <c r="R12">
-        <v>2259149</v>
-      </c>
-      <c r="S12" t="s">
-        <v>152</v>
-      </c>
-      <c r="T12" t="s">
-        <v>190</v>
-      </c>
-      <c r="U12" t="s">
-        <v>474</v>
-      </c>
-      <c r="V12" t="s">
-        <v>52</v>
-      </c>
-      <c r="W12">
-        <v>40011</v>
-      </c>
-      <c r="X12" t="s">
-        <v>475</v>
-      </c>
-      <c r="Y12">
-        <v>2197033</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>476</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>477</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD12">
-        <v>39519</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>478</v>
-      </c>
-      <c r="AF12">
-        <v>2259049</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>479</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>480</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>481</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK12">
-        <v>40005</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>482</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>483</v>
-      </c>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
@@ -4932,23 +4101,17 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AU5" r:id="rId1"/>
-    <hyperlink ref="AU7" r:id="rId2"/>
-    <hyperlink ref="AU6" r:id="rId3"/>
-    <hyperlink ref="AU9" r:id="rId4"/>
-    <hyperlink ref="AU10" r:id="rId5"/>
-    <hyperlink ref="AU11" r:id="rId6"/>
-    <hyperlink ref="AU12" r:id="rId7"/>
-    <hyperlink ref="AU8" r:id="rId8"/>
-    <hyperlink ref="AU4" r:id="rId9"/>
-    <hyperlink ref="AU2" r:id="rId10"/>
-    <hyperlink ref="AU3" r:id="rId11"/>
-    <hyperlink ref="J2" r:id="rId12"/>
-    <hyperlink ref="J3:J12" r:id="rId13" display="mario.es.ortega@gmail.com"/>
+    <hyperlink ref="AU6" r:id="rId2"/>
+    <hyperlink ref="AU4" r:id="rId3"/>
+    <hyperlink ref="AU2" r:id="rId4"/>
+    <hyperlink ref="AU3" r:id="rId5"/>
+    <hyperlink ref="J2" r:id="rId6"/>
+    <hyperlink ref="J3:J12" r:id="rId7" display="mario.es.ortega@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4981,7 +4144,7 @@
       </c>
       <c r="C3" s="9">
         <f>COUNTIF(Form_Responses[Categoría a participar],"Línea")</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4990,16 +4153,16 @@
       </c>
       <c r="C4" s="9">
         <f>COUNTIF(Form_Responses[Categoría a participar],"Laberinto")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>557</v>
+        <v>467</v>
       </c>
       <c r="C5" s="9">
         <f>SUM(C2:C4)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -5166,40 +4329,40 @@
         <v>46065.80955341435</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I2" s="7">
         <v>8126908090</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K2" s="7">
         <v>2244538</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>52</v>
@@ -5208,19 +4371,19 @@
         <v>39880</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="R2" s="7">
         <v>2244963</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>52</v>
@@ -5229,19 +4392,19 @@
         <v>39926</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Y2" s="7">
         <v>2293360</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AC2" s="7" t="s">
         <v>59</v>
@@ -5250,19 +4413,19 @@
         <v>40523</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AF2" s="7">
         <v>2293843</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AH2" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI2" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ2" s="7" t="s">
         <v>59</v>
@@ -5271,13 +4434,13 @@
         <v>40266</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AM2" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU2" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
@@ -5285,40 +4448,40 @@
         <v>46065.817240023149</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I3" s="7">
         <v>8126908090</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K3" s="7">
         <v>2291902</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>59</v>
@@ -5327,19 +4490,19 @@
         <v>40541</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R3" s="7">
         <v>2293459</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V3" s="7" t="s">
         <v>59</v>
@@ -5348,19 +4511,19 @@
         <v>40376</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Y3" s="7">
         <v>2291847</v>
       </c>
       <c r="Z3" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AC3" s="7" t="s">
         <v>59</v>
@@ -5369,19 +4532,19 @@
         <v>40415</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AF3" s="7">
         <v>2292039</v>
       </c>
       <c r="AG3" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AH3" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AI3" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="AJ3" s="7" t="s">
         <v>59</v>
@@ -5390,13 +4553,13 @@
         <v>40384</v>
       </c>
       <c r="AL3" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AM3" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU3" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
@@ -5404,40 +4567,40 @@
         <v>46065.82453006944</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I4" s="7">
         <v>8126908090</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K4" s="7">
         <v>2244761</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>52</v>
@@ -5446,19 +4609,19 @@
         <v>39899</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="R4" s="7">
         <v>2245057</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>52</v>
@@ -5467,19 +4630,19 @@
         <v>40018</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="Y4" s="7">
         <v>2293223</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="AC4" s="7" t="s">
         <v>59</v>
@@ -5488,19 +4651,19 @@
         <v>40351</v>
       </c>
       <c r="AE4" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="AF4" s="7">
         <v>2292527</v>
       </c>
       <c r="AG4" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AJ4" s="7" t="s">
         <v>59</v>
@@ -5509,7 +4672,7 @@
         <v>40411</v>
       </c>
       <c r="AL4" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="AM4" s="7" t="s">
         <v>60</v>
@@ -5518,13 +4681,13 @@
         <v>2293358</v>
       </c>
       <c r="AO4" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="AP4" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AQ4" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="AR4" s="7" t="s">
         <v>59</v>
@@ -5533,10 +4696,10 @@
         <v>40456</v>
       </c>
       <c r="AT4" s="7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="AU4" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -5544,40 +4707,40 @@
         <v>46065.72060119213</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I5" s="7">
         <v>8110506317</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K5" s="7">
         <v>2294408</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>59</v>
@@ -5586,19 +4749,19 @@
         <v>40208</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="R5" s="7">
         <v>2294422</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>59</v>
@@ -5607,19 +4770,19 @@
         <v>40462</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Y5" s="7">
         <v>2294172</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="AA5" s="7" t="s">
         <v>57</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="AC5" s="7" t="s">
         <v>59</v>
@@ -5628,19 +4791,19 @@
         <v>40540</v>
       </c>
       <c r="AE5" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AF5" s="7">
         <v>2294186</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AH5" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AI5" s="7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AJ5" s="7" t="s">
         <v>59</v>
@@ -5649,13 +4812,13 @@
         <v>40453</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="AM5" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU5" s="7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
@@ -5663,40 +4826,40 @@
         <v>46065.785894583329</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I6" s="7">
         <v>8181881065</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K6" s="7">
         <v>2259190</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>52</v>
@@ -5705,19 +4868,19 @@
         <v>40019</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="R6" s="7">
         <v>2259386</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>70</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>52</v>
@@ -5726,19 +4889,19 @@
         <v>40165</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Y6" s="7">
         <v>2259562</v>
       </c>
       <c r="Z6" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>52</v>
@@ -5747,34 +4910,34 @@
         <v>39935</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AF6" s="7">
         <v>2202397</v>
       </c>
       <c r="AG6" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AH6" s="7" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AI6" s="7" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="AJ6" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AK6" s="8">
         <v>39578</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="AM6" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU6" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.2">
@@ -5782,28 +4945,28 @@
         <v>46062.690090324075</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I7" s="7">
         <v>8113474496</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K7" s="7">
         <v>2233086</v>
@@ -5812,10 +4975,10 @@
         <v>49</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>52</v>
@@ -5824,19 +4987,19 @@
         <v>40058</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="R7" s="7">
         <v>2233367</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>52</v>
@@ -5845,19 +5008,19 @@
         <v>40166</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="Y7" s="7">
         <v>2262726</v>
       </c>
       <c r="Z7" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="AC7" s="7" t="s">
         <v>52</v>
@@ -5866,19 +5029,19 @@
         <v>39740</v>
       </c>
       <c r="AE7" s="7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AF7" s="7">
         <v>2262061</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AH7" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AI7" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AJ7" s="7" t="s">
         <v>52</v>
@@ -5887,13 +5050,13 @@
         <v>39963</v>
       </c>
       <c r="AL7" s="7" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="AM7" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU7" s="7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.2">
@@ -5901,40 +5064,40 @@
         <v>46062.700374097221</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I8" s="7">
         <v>8113474496</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K8" s="7">
         <v>2282526</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>59</v>
@@ -5943,19 +5106,19 @@
         <v>40443</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="R8" s="7">
         <v>2282616</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>59</v>
@@ -5964,19 +5127,19 @@
         <v>40318</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Y8" s="7">
         <v>2312367</v>
       </c>
       <c r="Z8" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AA8" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AB8" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>59</v>
@@ -5985,19 +5148,19 @@
         <v>40483</v>
       </c>
       <c r="AE8" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AF8" s="7">
         <v>2283341</v>
       </c>
       <c r="AG8" s="7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AH8" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="AI8" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AJ8" s="7" t="s">
         <v>59</v>
@@ -6006,7 +5169,7 @@
         <v>39926</v>
       </c>
       <c r="AL8" s="7" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AM8" s="7" t="s">
         <v>60</v>
@@ -6015,13 +5178,13 @@
         <v>2283289</v>
       </c>
       <c r="AO8" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="AP8" s="7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AQ8" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AR8" s="7" t="s">
         <v>59</v>
@@ -6030,10 +5193,10 @@
         <v>40303</v>
       </c>
       <c r="AT8" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AU8" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.2">
@@ -6041,40 +5204,40 @@
         <v>46065.395366539349</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I9" s="7">
         <v>8113474496</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K9" s="7">
         <v>2312840</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>59</v>
@@ -6083,19 +5246,19 @@
         <v>40386</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="R9" s="7">
         <v>2312938</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>59</v>
@@ -6104,19 +5267,19 @@
         <v>40353</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="Y9" s="7">
         <v>2312939</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AA9" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AB9" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="AC9" s="7" t="s">
         <v>59</v>
@@ -6125,19 +5288,19 @@
         <v>40462</v>
       </c>
       <c r="AE9" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="AF9" s="7">
         <v>2282538</v>
       </c>
       <c r="AG9" s="7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="AH9" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="AI9" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AJ9" s="7" t="s">
         <v>59</v>
@@ -6146,13 +5309,13 @@
         <v>40343</v>
       </c>
       <c r="AL9" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AM9" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU9" s="7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.2">
@@ -6160,19 +5323,19 @@
         <v>46065.346729571756</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>51</v>
@@ -6181,40 +5344,40 @@
         <v>8180889179</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="K10" s="7">
         <v>2203980</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P10" s="8">
         <v>39569</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="R10" s="7">
         <v>2311083</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>59</v>
@@ -6223,19 +5386,19 @@
         <v>40435</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="Y10" s="7">
         <v>2311109</v>
       </c>
       <c r="Z10" s="7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="AA10" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="AB10" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AC10" s="7" t="s">
         <v>59</v>
@@ -6244,19 +5407,19 @@
         <v>40255</v>
       </c>
       <c r="AE10" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AF10" s="7">
         <v>2310886</v>
       </c>
       <c r="AG10" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AH10" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="AI10" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="AJ10" s="7" t="s">
         <v>59</v>
@@ -6265,13 +5428,13 @@
         <v>40432</v>
       </c>
       <c r="AL10" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AM10" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU10" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.2">
@@ -6279,19 +5442,19 @@
         <v>46065.350905219908</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>51</v>
@@ -6300,28 +5463,28 @@
         <v>8180889179</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="K11" s="7">
         <v>2204196</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>68</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P11" s="8">
         <v>39603</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="R11" s="7">
         <v>2203806</v>
@@ -6330,52 +5493,52 @@
         <v>65</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W11" s="8">
         <v>39481</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="Y11" s="7">
         <v>2203988</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AB11" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AD11" s="8">
         <v>39730</v>
       </c>
       <c r="AE11" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="AF11" s="7">
         <v>2311158</v>
       </c>
       <c r="AG11" s="7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="AH11" s="7" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="AI11" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="AJ11" s="7" t="s">
         <v>59</v>
@@ -6384,13 +5547,13 @@
         <v>40361</v>
       </c>
       <c r="AL11" s="7" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="AM11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU11" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.2">
@@ -6398,40 +5561,40 @@
         <v>46065.362685763888</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I12" s="7">
         <v>8116013233</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="K12" s="7">
         <v>2260899</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>52</v>
@@ -6440,19 +5603,19 @@
         <v>39973</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="R12" s="7">
         <v>2260905</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="T12" s="7" t="s">
         <v>57</v>
       </c>
       <c r="U12" s="7" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="V12" s="7" t="s">
         <v>52</v>
@@ -6461,19 +5624,19 @@
         <v>40016</v>
       </c>
       <c r="X12" s="7" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="Y12" s="7">
         <v>2260827</v>
       </c>
       <c r="Z12" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AA12" s="7" t="s">
         <v>65</v>
       </c>
       <c r="AB12" s="7" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="AC12" s="7" t="s">
         <v>52</v>
@@ -6482,19 +5645,19 @@
         <v>40163</v>
       </c>
       <c r="AE12" s="7" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="AF12" s="7">
         <v>2311249</v>
       </c>
       <c r="AG12" s="7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="AI12" s="7" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="AJ12" s="7" t="s">
         <v>59</v>
@@ -6503,7 +5666,7 @@
         <v>40270</v>
       </c>
       <c r="AL12" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="AM12" s="7" t="s">
         <v>60</v>
@@ -6515,10 +5678,10 @@
         <v>67</v>
       </c>
       <c r="AP12" s="7" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="AQ12" s="7" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AR12" s="7" t="s">
         <v>59</v>
@@ -6527,10 +5690,10 @@
         <v>40524</v>
       </c>
       <c r="AT12" s="7" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="AU12" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.2">
@@ -6538,40 +5701,40 @@
         <v>46064.644861875</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I13" s="7">
         <v>8112698855</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K13" s="7">
         <v>2246494</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>52</v>
@@ -6580,19 +5743,19 @@
         <v>39911</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="R13" s="7">
         <v>2246376</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>52</v>
@@ -6601,40 +5764,40 @@
         <v>39818</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="Y13" s="7">
         <v>2184652</v>
       </c>
       <c r="Z13" s="7" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="AA13" s="7" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AB13" s="7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AD13" s="8">
         <v>39758</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="AF13" s="7">
         <v>2305317</v>
       </c>
       <c r="AG13" s="7" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="AH13" s="7" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="AI13" s="7" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="AJ13" s="7" t="s">
         <v>59</v>
@@ -6643,7 +5806,7 @@
         <v>40469</v>
       </c>
       <c r="AL13" s="7" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="AM13" s="7" t="s">
         <v>60</v>
@@ -6652,13 +5815,13 @@
         <v>2305939</v>
       </c>
       <c r="AO13" s="7" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="AP13" s="7" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="AQ13" s="7" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="AR13" s="7" t="s">
         <v>59</v>
@@ -6667,10 +5830,10 @@
         <v>40247</v>
       </c>
       <c r="AT13" s="7" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="AU13" s="7" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.2">
@@ -6678,61 +5841,61 @@
         <v>46064.647735729166</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I14" s="7">
         <v>8112698855</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K14" s="7">
         <v>2184367</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P14" s="8">
         <v>39572</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="R14" s="7">
         <v>2305793</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>59</v>
@@ -6741,19 +5904,19 @@
         <v>40243</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="Y14" s="7">
         <v>2305379</v>
       </c>
       <c r="Z14" s="7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="AA14" s="7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="AB14" s="7" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="AC14" s="7" t="s">
         <v>59</v>
@@ -6762,19 +5925,19 @@
         <v>40405</v>
       </c>
       <c r="AE14" s="7" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="AF14" s="7">
         <v>2305698</v>
       </c>
       <c r="AG14" s="7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AH14" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="AI14" s="7" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AJ14" s="7" t="s">
         <v>59</v>
@@ -6783,13 +5946,13 @@
         <v>40366</v>
       </c>
       <c r="AL14" s="7" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="AM14" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AU14" s="7" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -6809,43 +5972,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>524</v>
+        <v>434</v>
       </c>
       <c r="B1" t="s">
-        <v>525</v>
+        <v>435</v>
       </c>
       <c r="C1" t="s">
-        <v>508</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>487</v>
+        <v>408</v>
       </c>
       <c r="B4" t="s">
-        <v>488</v>
+        <v>409</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
@@ -6853,43 +6016,43 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>442</v>
+        <v>399</v>
       </c>
       <c r="B6" t="s">
-        <v>457</v>
+        <v>403</v>
       </c>
       <c r="C6" t="s">
-        <v>458</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>469</v>
+        <v>405</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>470</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
@@ -6897,76 +6060,76 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>412</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -7018,29 +6181,29 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B21" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C21" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>484</v>
+        <v>407</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
@@ -7051,65 +6214,65 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>454</v>
+        <v>402</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>452</v>
+        <v>400</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>500</v>
+        <v>410</v>
       </c>
       <c r="B25" t="s">
-        <v>501</v>
+        <v>411</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
         <v>61</v>
@@ -7117,24 +6280,24 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B29" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C29" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>